<commit_message>
- Switching from Ray Tune to Optuna - former has shit Windows support, blue screens. Wrapped existing tune methods in optuna functionality. Reworked the experimental script and model_tuner.py.  - Model.py: Separated make_model_like and get_model_type  - Added static methods to suggest values for an optuna trial: EHD_Model.optuna_init(); RF_Classifier_Allpre.optuna_suggest(trial)
</commit_message>
<xml_diff>
--- a/tests/patch_test_files/measurements.xlsx
+++ b/tests/patch_test_files/measurements.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
print-day additions. Need to make this independent from gridgraph
</commit_message>
<xml_diff>
--- a/tests/patch_test_files/measurements.xlsx
+++ b/tests/patch_test_files/measurements.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Added several transfer models
</commit_message>
<xml_diff>
--- a/tests/patch_test_files/measurements.xlsx
+++ b/tests/patch_test_files/measurements.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>